<commit_message>
nutrient composition for composite categories now read in from spreadsheets for each composite category.
df.nutrients converted to data table and called dt.nutrients
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/nutrientDetails/comp_recalc_c_Crust_crustaceans_FCT_EPC_012916.xlsx
+++ b/data-raw/NutrientData/nutrientDetails/comp_recalc_c_Crust_crustaceans_FCT_EPC_012916.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-30320" yWindow="-3420" windowWidth="28800" windowHeight="12440"/>
+    <workbookView xWindow="-30320" yWindow="-3420" windowWidth="28800" windowHeight="12440" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="c_Crust" sheetId="1" r:id="rId1"/>
@@ -2052,7 +2052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -16015,9 +16015,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>